<commit_message>
payment confirmation from yoomoney
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Прочее\YandexDisk\11\project\Marketplace_prod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Диски\YandexDisk\11\project\Marketplace_prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA00F397-6C04-4E27-87ED-56FF9F27F468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2C2A3A-2C0E-4255-BDF8-FAB0CD62B9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="89">
   <si>
     <t>Заголовок</t>
   </si>
@@ -296,6 +295,18 @@
   </si>
   <si>
     <t>sub3</t>
+  </si>
+  <si>
+    <t>Мужчины</t>
+  </si>
+  <si>
+    <t>Инопланетянин</t>
+  </si>
+  <si>
+    <t>Антигель AVS AVK-167, 340 мл 2 шт</t>
+  </si>
+  <si>
+    <t>Инопланетянин212312</t>
   </si>
 </sst>
 </file>
@@ -656,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,6 +779,9 @@
       <c r="D2" t="s">
         <v>56</v>
       </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
       <c r="F2" t="s">
         <v>57</v>
       </c>
@@ -1191,6 +1205,9 @@
       <c r="D14" t="s">
         <v>41</v>
       </c>
+      <c r="E14" t="s">
+        <v>86</v>
+      </c>
       <c r="F14" t="s">
         <v>49</v>
       </c>
@@ -1251,6 +1268,47 @@
         <v>24</v>
       </c>
       <c r="M15" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16">
+        <v>269</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16">
+        <v>100</v>
+      </c>
+      <c r="J16" t="s">
+        <v>53</v>
+      </c>
+      <c r="K16" t="s">
+        <v>54</v>
+      </c>
+      <c r="L16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>